<commit_message>
Modifs Backlog et Charte
</commit_message>
<xml_diff>
--- a/Backlog projet annuel.xlsx
+++ b/Backlog projet annuel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L3 2016-2017\Projet Annuel\Projet-annuel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="13935" windowHeight="8715"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>N°</t>
   </si>
@@ -31,26 +36,32 @@
     <t>Une camera peut reconnaitre un plateau</t>
   </si>
   <si>
-    <t>Une camera peut lire un QR code et lui associer une image 2D</t>
-  </si>
-  <si>
     <t>Un joueur peut jouer contre un autre joueur avec des QR codes</t>
   </si>
   <si>
     <t>Un joueur peut parametrer sa partie avec des QR codes</t>
   </si>
   <si>
-    <t>Un joueur peut lire les coups joués par une IA,et actualiser l'etat de son plateau physique</t>
-  </si>
-  <si>
     <t>Un joueur peut jouer contre une IA</t>
+  </si>
+  <si>
+    <t>Une camera peut lire un QR code et lui superposer une image 2D</t>
+  </si>
+  <si>
+    <t>L'application peut vérifier la validité des coups joués</t>
+  </si>
+  <si>
+    <t>L'application marque les pions éliminés d'une croix</t>
+  </si>
+  <si>
+    <t>L'application ne prend pas de coup en compte tant que le joueur ne retire pas les pions marqués</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,34 +114,34 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -138,15 +149,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:D8" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:D7"/>
-  <sortState ref="A2:D7">
-    <sortCondition ref="C1:C7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:D10" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:D9"/>
+  <sortState ref="A2:D9">
+    <sortCondition ref="C1:C9"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="2" name="N°" dataDxfId="7" totalsRowDxfId="3"/>
@@ -159,7 +173,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -201,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +247,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +282,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,26 +458,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="51.75" customWidth="1"/>
-    <col min="3" max="3" width="10.75" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.375" style="2"/>
+    <col min="2" max="2" width="68" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,12 +491,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -489,7 +505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>3</v>
       </c>
@@ -503,81 +519,109 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="5">
-        <v>6</v>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
         <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>